<commit_message>
okie. getting it to a good place to come back to.
</commit_message>
<xml_diff>
--- a/output/FUTURA-System-Manual.xlsx
+++ b/output/FUTURA-System-Manual.xlsx
@@ -3408,7 +3408,6 @@
     <row r="236">
       <c r="A236" t="inlineStr"/>
       <c r="B236" t="inlineStr"/>
-      <c r="C236" t="inlineStr"/>
       <c r="D236" t="inlineStr"/>
       <c r="E236" t="inlineStr">
         <is>
@@ -3427,7 +3426,6 @@
           <t>0 V DC</t>
         </is>
       </c>
-      <c r="C237" t="inlineStr"/>
       <c r="D237" t="inlineStr">
         <is>
           <t>8</t>
@@ -3450,7 +3448,6 @@
           <t>24 V DC</t>
         </is>
       </c>
-      <c r="C238" t="inlineStr"/>
       <c r="D238" t="inlineStr">
         <is>
           <t>9</t>
@@ -3465,7 +3462,6 @@
     <row r="239">
       <c r="A239" t="inlineStr"/>
       <c r="B239" t="inlineStr"/>
-      <c r="C239" t="inlineStr"/>
       <c r="D239" t="inlineStr">
         <is>
           <t>10</t>
@@ -3488,7 +3484,6 @@
           <t>Reserved, do not use</t>
         </is>
       </c>
-      <c r="C240" t="inlineStr"/>
       <c r="D240" t="inlineStr">
         <is>
           <t>11</t>
@@ -3506,7 +3501,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="C241" t="inlineStr"/>
       <c r="D241" t="inlineStr"/>
       <c r="E241" t="inlineStr"/>
     </row>
@@ -3516,7 +3510,6 @@
           <t>5</t>
         </is>
       </c>
-      <c r="C242" t="inlineStr"/>
       <c r="D242" t="inlineStr"/>
       <c r="E242" t="inlineStr">
         <is>
@@ -3530,7 +3523,6 @@
           <t>6</t>
         </is>
       </c>
-      <c r="C243" t="inlineStr"/>
       <c r="D243" t="inlineStr">
         <is>
           <t>12</t>
@@ -3548,7 +3540,6 @@
           <t>7</t>
         </is>
       </c>
-      <c r="C244" t="inlineStr"/>
       <c r="D244" t="inlineStr">
         <is>
           <t>13</t>
@@ -3563,7 +3554,6 @@
     <row r="245">
       <c r="A245" t="inlineStr"/>
       <c r="B245" t="inlineStr"/>
-      <c r="C245" t="inlineStr"/>
       <c r="D245" t="inlineStr">
         <is>
           <t>14</t>

</xml_diff>